<commit_message>
Added onboard admin config instructions
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hayden\Documents\Orcinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F903B6AD-69C3-489A-9200-562FC637DB08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1B0ECD-49EE-4AFE-BFFB-5385E73D6BD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{E8B8B465-02C2-405B-95CA-32F45BF1045B}"/>
+    <workbookView xWindow="1275" yWindow="2460" windowWidth="21600" windowHeight="11423" xr2:uid="{E8B8B465-02C2-405B-95CA-32F45BF1045B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>Orcinus Inventory</t>
   </si>
@@ -244,9 +246,6 @@
   </si>
   <si>
     <t>Theory lab, boxed</t>
-  </si>
-  <si>
-    <t>Note: replace blades on chassis 16 and 10 LAST</t>
   </si>
   <si>
     <t>Theory lab</t>
@@ -636,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4488E0-15B5-48AC-BD83-4630A661A86F}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -944,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
         <v>48</v>
@@ -961,7 +960,7 @@
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
@@ -975,7 +974,7 @@
         <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
@@ -1042,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
         <v>63</v>
@@ -1074,11 +1073,6 @@
       </c>
       <c r="D32" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>